<commit_message>
picture size in Forum
</commit_message>
<xml_diff>
--- a/ruby.xlsx
+++ b/ruby.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="560" yWindow="1640" windowWidth="28240" windowHeight="12000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="560" yWindow="1640" windowWidth="28240" windowHeight="14360" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="86">
   <si>
     <t>https://www.youtube.com/watch?v=4nyzl3pVXp4</t>
   </si>
@@ -280,6 +280,9 @@
   </si>
   <si>
     <t>git commit - am "blabla"</t>
+  </si>
+  <si>
+    <t>git status</t>
   </si>
 </sst>
 </file>
@@ -895,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F17" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1201,6 +1204,9 @@
       <c r="I32" t="s">
         <v>70</v>
       </c>
+      <c r="O32" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="33" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C33" t="s">

</xml_diff>

<commit_message>
website non editable for non admin safety
</commit_message>
<xml_diff>
--- a/ruby.xlsx
+++ b/ruby.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="159">
   <si>
     <t>https://www.youtube.com/watch?v=4nyzl3pVXp4</t>
   </si>
@@ -497,6 +497,12 @@
   </si>
   <si>
     <t>git add .</t>
+  </si>
+  <si>
+    <t>heroku run rake db:migrate</t>
+  </si>
+  <si>
+    <t>heroku run rails console</t>
   </si>
 </sst>
 </file>
@@ -1115,7 +1121,7 @@
   <dimension ref="B3:Y72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+      <selection activeCell="R39" sqref="R39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1477,10 +1483,18 @@
       <c r="I36" t="s">
         <v>73</v>
       </c>
+      <c r="R36" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="37" spans="3:18" x14ac:dyDescent="0.2">
       <c r="I37" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="R38" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="67" spans="14:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
remove render for bike
</commit_message>
<xml_diff>
--- a/ruby.xlsx
+++ b/ruby.xlsx
@@ -13,8 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="bike" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="edit tips" sheetId="2" r:id="rId2"/>
+    <sheet name="bike list" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -1120,7 +1120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
       <selection activeCell="R39" sqref="R39"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
remove picture from forum
</commit_message>
<xml_diff>
--- a/ruby.xlsx
+++ b/ruby.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="4080" yWindow="5080" windowWidth="26260" windowHeight="17560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="162">
   <si>
     <t>https://www.youtube.com/watch?v=4nyzl3pVXp4</t>
   </si>
@@ -503,6 +503,15 @@
   </si>
   <si>
     <t>heroku run rails console</t>
+  </si>
+  <si>
+    <t>photo</t>
+  </si>
+  <si>
+    <t>Suzuki.ca</t>
+  </si>
+  <si>
+    <t>q.remove_pictureintro!</t>
   </si>
 </sst>
 </file>
@@ -1120,8 +1129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="R39" sqref="R39"/>
+    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1493,6 +1502,9 @@
       </c>
     </row>
     <row r="38" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="J38" t="s">
+        <v>161</v>
+      </c>
       <c r="R38" t="s">
         <v>158</v>
       </c>
@@ -1535,339 +1547,345 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AG10"/>
+  <dimension ref="A2:AH10"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="12.33203125" customWidth="1"/>
-    <col min="20" max="20" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.1640625" customWidth="1"/>
-    <col min="22" max="22" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="12.33203125" customWidth="1"/>
+    <col min="21" max="21" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.1640625" customWidth="1"/>
+    <col min="23" max="23" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="L2" t="s">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="L3" t="s">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="M3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>89</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>95</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>29</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>90</v>
       </c>
-      <c r="C5">
+      <c r="B5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D5">
         <v>1300</v>
-      </c>
-      <c r="D5">
-        <v>1000</v>
       </c>
       <c r="E5">
         <v>1000</v>
       </c>
       <c r="F5">
+        <v>1000</v>
+      </c>
+      <c r="G5">
         <v>750</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>600</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>400</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>250</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>1250</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>1000</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>900</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>750</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>650</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>300</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>125</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>1200</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>1000</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>750</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>650</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>500</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>300</v>
       </c>
-      <c r="Z5">
+      <c r="AA5">
         <v>1800</v>
       </c>
-      <c r="AA5">
+      <c r="AB5">
         <v>1462</v>
-      </c>
-      <c r="AB5">
-        <v>1300</v>
       </c>
       <c r="AC5">
         <v>1300</v>
       </c>
-      <c r="AE5">
+      <c r="AD5">
+        <v>1300</v>
+      </c>
+      <c r="AF5">
         <v>900</v>
       </c>
-      <c r="AF5">
+      <c r="AG5">
         <v>650</v>
       </c>
-      <c r="AG5">
+      <c r="AH5">
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>54</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D6" t="s">
         <v>53</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>97</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>98</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>99</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>100</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>96</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>93</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>94</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>92</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>103</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>101</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>104</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>105</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>106</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>107</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>108</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>109</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>110</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>111</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>113</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>112</v>
       </c>
       <c r="AD7" t="s">
         <v>112</v>
       </c>
-      <c r="AF7" t="s">
+      <c r="AE7" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG7" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>115</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>118</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>116</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>117</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>120</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>119</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>121</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>122</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>123</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>124</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>125</v>
       </c>
-      <c r="V8" t="s">
+      <c r="W8" t="s">
         <v>126</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>127</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AA8" t="s">
         <v>128</v>
       </c>
-      <c r="AE8" t="s">
+      <c r="AF8" t="s">
         <v>130</v>
       </c>
-      <c r="AF8" t="s">
+      <c r="AG8" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>131</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>133</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>132</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>134</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>135</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>136</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>137</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>138</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>142</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AC9" t="s">
         <v>141</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AF9" t="s">
         <v>139</v>
       </c>
-      <c r="AG9" t="s">
+      <c r="AH9" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
         <v>145</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>144</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>143</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>146</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>153</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>43</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>147</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>148</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>149</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
         <v>150</v>
       </c>
-      <c r="U10" t="s">
+      <c r="V10" t="s">
         <v>151</v>
       </c>
-      <c r="V10" t="s">
+      <c r="W10" t="s">
         <v>152</v>
       </c>
     </row>

</xml_diff>

<commit_message>
index bike add info
</commit_message>
<xml_diff>
--- a/ruby.xlsx
+++ b/ruby.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maverick/Antoine/site web/full_throttle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{14B2D9DD-7870-194B-BED5-4FFAD03BD42E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{09F99130-9A41-D748-9563-0C9F0E5D975A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="4740" windowWidth="26260" windowHeight="12820" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1183,7 +1183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:Y72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E21" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G16" workbookViewId="0">
       <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>

</xml_diff>